<commit_message>
optimized activity,video actions and set min limit to user input
</commit_message>
<xml_diff>
--- a/actions/PMT_actions_2023_05_09.xlsx
+++ b/actions/PMT_actions_2023_05_09.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,24 +420,21 @@
         <v>Age</v>
       </c>
       <c r="F1" t="str">
-        <v>User input</v>
+        <v>Media</v>
       </c>
       <c r="G1" t="str">
-        <v>Media</v>
+        <v>Content</v>
       </c>
       <c r="H1" t="str">
-        <v>Content</v>
+        <v>Alternative Content</v>
       </c>
       <c r="I1" t="str">
-        <v>Alternative Content</v>
+        <v>Source content</v>
       </c>
       <c r="J1" t="str">
-        <v>Source content</v>
+        <v>Inspiration</v>
       </c>
       <c r="K1" t="str">
-        <v>Inspiration</v>
-      </c>
-      <c r="L1" t="str">
         <v>Comments</v>
       </c>
     </row>
@@ -452,16 +449,13 @@
         <v>Consequences of smoking - General</v>
       </c>
       <c r="F2" t="str">
-        <v>True</v>
-      </c>
-      <c r="G2" t="str">
-        <v>text</v>
-      </c>
-      <c r="H2" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G2" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking has many disadvantages and risks but on the long-run it is quite unhealthy for your body. Choose a topic to find out more:
 physical health;heart diseases;appearance;oral health;respiratory illnesses;life expectancy;fertility</v>
       </c>
-      <c r="I2" t="str" xml:space="preserve">
+      <c r="H2" t="str" xml:space="preserve">
         <v xml:space="preserve">The dangers of smoking are extensive and can have severe consequences for your health. If you continue to smoke, you increase your risk of developing a range of health problems that can significantly impact your quality of life. Choose a topic to find out more:
 physical health; heart diseases; appearance; oral health; respiratory illnesses; life expectancy; fertility</v>
       </c>
@@ -476,21 +470,21 @@
       <c r="C3" t="str">
         <v>Physical health</v>
       </c>
-      <c r="G3" t="str">
-        <v>text</v>
-      </c>
-      <c r="H3" t="str" xml:space="preserve">
+      <c r="F3" t="str">
+        <v>text</v>
+      </c>
+      <c r="G3" t="str" xml:space="preserve">
         <v xml:space="preserve">Firstly, smoking can have a significant impact on your physical health. 
 It can cause your condition to deteriorate, leaving you with less energy and strength. 
 You'll get tired faster and pant more often, limiting your ability to enjoy physical activities.</v>
       </c>
+      <c r="I3" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J3" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K3" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L3" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -504,20 +498,20 @@
       <c r="C4" t="str">
         <v>Heart diseases</v>
       </c>
-      <c r="G4" t="str">
-        <v>text</v>
-      </c>
-      <c r="H4" t="str" xml:space="preserve">
+      <c r="F4" t="str">
+        <v>text</v>
+      </c>
+      <c r="G4" t="str" xml:space="preserve">
         <v xml:space="preserve">Perhaps most concerning, smoking can increase your risk of developing severe heart and blood vessel diseases, including stroke and heart attack. 
 Smoking can also increase your risk of developing various types of cancer, including lung, throat, esophageal, pancreatic, bladder, kidney, and cervical cancer in women.</v>
       </c>
+      <c r="I4" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J4" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K4" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L4" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -531,21 +525,21 @@
       <c r="C5" t="str">
         <v>Appearance</v>
       </c>
-      <c r="G5" t="str">
-        <v>text</v>
-      </c>
-      <c r="H5" t="str" xml:space="preserve">
+      <c r="F5" t="str">
+        <v>text</v>
+      </c>
+      <c r="G5" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can have a negative effect on your appearance. 
 You also run the risk that your skin looks less healthy and that you look older and/or tired as a result. You also run the risk that your hair loses shine, turns grey faster, or experiences hair loss altogether. 
 Additionally, it is often the case that the odor of smoke clings to your clothes, hair, and home, which can leave you smelling unpleasant and unclean.</v>
       </c>
+      <c r="I5" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J5" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K5" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L5" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -559,22 +553,22 @@
       <c r="C6" t="str">
         <v>Oral health</v>
       </c>
-      <c r="G6" t="str">
-        <v>text</v>
-      </c>
-      <c r="H6" t="str" xml:space="preserve">
+      <c r="F6" t="str">
+        <v>text</v>
+      </c>
+      <c r="G6" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can also damage your oral health. 
 Your teeth may become yellow or brown, and you're more likely to experience inflamed gums. 
 You may also develop a hoarse voice, catch colds more often, and experience inflammation in your nose, sinuses, throat, and ears.
 This can lead to sore throats, earaches, and headaches.</v>
       </c>
+      <c r="I6" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J6" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K6" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L6" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -588,20 +582,20 @@
       <c r="C7" t="str">
         <v>Respiratory illnesses</v>
       </c>
-      <c r="G7" t="str">
-        <v>text</v>
-      </c>
-      <c r="H7" t="str" xml:space="preserve">
+      <c r="F7" t="str">
+        <v>text</v>
+      </c>
+      <c r="G7" t="str" xml:space="preserve">
         <v xml:space="preserve">Perhaps most concerning, smoking can increase your risk of developing serious respiratory illnesses such as asthma, bronchitis, and pneumonia. 
 These conditions can cause mucus, coughing, and tightness in your chest, which can be uncomfortable and limit your ability to enjoy life to the fullest.</v>
       </c>
+      <c r="I7" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J7" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K7" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L7" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -615,20 +609,20 @@
       <c r="C8" t="str">
         <v>Life expectancy</v>
       </c>
-      <c r="G8" t="str">
-        <v>text</v>
-      </c>
-      <c r="H8" t="str" xml:space="preserve">
+      <c r="F8" t="str">
+        <v>text</v>
+      </c>
+      <c r="G8" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can significantly shorten your life expectancy. 
 People who smoke every day die on average 10 years earlier than non-smokers, but not smoking can reverse a lot of the negative health outcomes of smoking.</v>
       </c>
+      <c r="I8" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J8" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K8" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L8" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -642,20 +636,20 @@
       <c r="C9" t="str">
         <v>Fertility</v>
       </c>
-      <c r="G9" t="str">
-        <v>text</v>
-      </c>
-      <c r="H9" t="str" xml:space="preserve">
+      <c r="F9" t="str">
+        <v>text</v>
+      </c>
+      <c r="G9" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can negatively impact your fertility. 
 Smoking can, for example, lead to erectile dysfunction or difficulties to achieve pregnancy.</v>
       </c>
+      <c r="I9" t="str">
+        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+      </c>
       <c r="J9" t="str">
-        <v>https://www.thuisarts.nl/stoppen-met-roken/ik-wil-misschien-stoppen-met-roken-0</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K9" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L9" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -670,12 +664,9 @@
         <v>Consequences of smoking - Cancer</v>
       </c>
       <c r="F10" t="str">
-        <v>True</v>
-      </c>
-      <c r="G10" t="str">
-        <v>text</v>
-      </c>
-      <c r="H10" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G10" t="str" xml:space="preserve">
         <v xml:space="preserve">Can you estimate how many deaths per year worldwide are caused by tobacco use?
 10%;25%;40%</v>
       </c>
@@ -690,21 +681,21 @@
       <c r="C11" t="str">
         <v>Consequences of smoking - Cancer</v>
       </c>
-      <c r="G11" t="str">
-        <v>text</v>
-      </c>
-      <c r="H11" t="str" xml:space="preserve">
+      <c r="F11" t="str">
+        <v>text</v>
+      </c>
+      <c r="G11" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking is detrimental for your health' The act of smoking poses numerous drawbacks and hazards, including cancer.
 Did you know that every year, according to the World Health Organization (WHO), tobacco use is responsible for approximately 25% of all cancer deaths worldwide?! This translates to around 1.7 million cancer deaths per year globally.
 Smoking causes various types of cancer. The carcinogenic substances from smoke are absorbed into your blood and spread throughout the body. Therefore, smoking can cause cancer anywhere in your body.</v>
       </c>
+      <c r="I11" t="str">
+        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+      </c>
       <c r="J11" t="str">
-        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K11" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L11" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -719,12 +710,9 @@
         <v>Consequences of smoking - Heart and vascular disease</v>
       </c>
       <c r="F12" t="str">
-        <v>True</v>
-      </c>
-      <c r="G12" t="str">
-        <v>text</v>
-      </c>
-      <c r="H12" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G12" t="str" xml:space="preserve">
         <v xml:space="preserve">You know that smoking is terrible. Did you know, though, that it can cause heart and vascular diseases?
 yes;no</v>
       </c>
@@ -739,16 +727,16 @@
       <c r="C13" t="str">
         <v>Consequences of smoking - Heart and vascular disease</v>
       </c>
-      <c r="G13" t="str">
-        <v>text</v>
-      </c>
-      <c r="H13" t="str" xml:space="preserve">
+      <c r="F13" t="str">
+        <v>text</v>
+      </c>
+      <c r="G13" t="str" xml:space="preserve">
         <v xml:space="preserve">Certain substances in tobacco smoke, such as nicotine, damage the inside of blood vessels and make them rough. The body reacts to this the same way it does to wounds on your skin: scabs are made.
 These scabs slowly clog the blood vessels. This prevents the blood from passing through them properly. The vessels themselves become less flexible and rupture more easily.
 Also, part of the thickening can break off and clog a blood vessel further down. This process is called atherosclerosis (arteriosclerosis).
 Therefore, smoking can cause various heart and vascular diseases in your body.</v>
       </c>
-      <c r="I13" t="str" xml:space="preserve">
+      <c r="H13" t="str" xml:space="preserve">
         <v xml:space="preserve">Nicotine gives the body a brief "kick" in which blood pressure is raised. High blood pressure is especially risky if the vessels are weak. This puts smokers at increased risk for cardiovascular diseases, such as:
 High blood pressure: Nicotine constricts blood vessels and causes higher blood pressure. Smoking when blood pressure is already too high is, therefore, extra harmful to blood vessels. Medications for high blood pressure do not work as well in smokers.
 Damage to blood vessels: The changes in blood vessels can lead to "smoker's legs. People with 'smoker's legs' experience discomfort in their legs after only a short walk. They then have to stand still for a while until the pain goes away. 
@@ -756,13 +744,13 @@
 Heart attack: In a heart attack, the heart no longer receives oxygen. This is because the blood vessels that carry oxygen to the heart are blocked. Smokers are 2 times more likely to have a heart attack.
 Stroke: Smokers are more likely to have a stroke than people who don't smoke. This is due to high blood pressure and changes in blood vessels in the brain. There are two types of stroke: cerebral haemorrhage and cerebral infarction. In a brain haemorrhage, a blood vessel in the brain breaks. A blood clot causes a blood vessel in the brain to close in a cerebral infarction.</v>
       </c>
+      <c r="I13" t="str">
+        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+      </c>
       <c r="J13" t="str">
-        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K13" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L13" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -777,12 +765,9 @@
         <v>Consequences of smoking -  Lung diseases</v>
       </c>
       <c r="F14" t="str">
-        <v>True</v>
-      </c>
-      <c r="G14" t="str">
-        <v>text</v>
-      </c>
-      <c r="H14" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G14" t="str" xml:space="preserve">
         <v xml:space="preserve">What do you think it's the deathliest form of cancer? 
 lung cancer; colorectar cancer; breast cancer</v>
       </c>
@@ -797,27 +782,27 @@
       <c r="C15" t="str">
         <v>Consequences of smoking -  Lung diseases</v>
       </c>
-      <c r="G15" t="str">
-        <v>text</v>
-      </c>
-      <c r="H15" t="str" xml:space="preserve">
+      <c r="F15" t="str">
+        <v>text</v>
+      </c>
+      <c r="G15" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking is the leading cause of lung disease. Common lung diseases are lung cancer and COPD. Smoking kills more than 6,000 people from COPD and 10,000 from lung cancer every year, making it the deathliest form of cancer.
 The lungs contain cilia that keep them clean. Because of the tar in cigarettes, cilia stick together. The cilia can then no longer do their job properly.
 Smoking also makes the lungs dirtier and irritates the mucous membranes in the lungs. Chronic inflammation can develop.
 When the cilia can no longer dispose of mucus, the only way to do so is by coughing (smoker's cough). So the body's way of keeping itself clean and healthy is disrupted by smoking.</v>
       </c>
-      <c r="I15" t="str" xml:space="preserve">
+      <c r="H15" t="str" xml:space="preserve">
         <v xml:space="preserve">COPD is an English abbreviation and means Chronic Obstructive Pulmonary Diseases. COPD is a collective name for chronic bronchitis and emphysema. In chronic bronchitis, the airways are narrowed due to inflammation. In emphysema, the lungs are damaged. It causes severe shortness of breath, coughing, fatigue and difficulty breathing. 
 Every year, more than 6,000 people die from COPD. Of these deaths, 80% are caused by smoking.
 Lung cancer causes 10,000 deaths annually, making it the deadliest form of cancer. Asthma can be caused and aggravated by smoking. Secondhand smoke also has this effect, especially in children.</v>
       </c>
+      <c r="I15" t="str">
+        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+      </c>
       <c r="J15" t="str">
-        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K15" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L15" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -832,12 +817,9 @@
         <v>Consequences of smoking -  Lung diseases</v>
       </c>
       <c r="F16" t="str">
-        <v>True</v>
-      </c>
-      <c r="G16" t="str">
-        <v>text</v>
-      </c>
-      <c r="H16" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G16" t="str" xml:space="preserve">
         <v xml:space="preserve">Did you know that blindness and certain eye conditions are more common in smokers than in nonsmokers?
 yes;no</v>
       </c>
@@ -852,22 +834,22 @@
       <c r="C17" t="str">
         <v>Consequences of smoking - Eye diseases</v>
       </c>
-      <c r="G17" t="str">
-        <v>text</v>
-      </c>
-      <c r="H17" t="str" xml:space="preserve">
+      <c r="F17" t="str">
+        <v>text</v>
+      </c>
+      <c r="G17" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can cause eye diseases such as macular degeneration, glaucoma and cataract.
 With macular degeneration (MD), you can no longer see sharply in the centre of your vision. The risk of macular degeneration increases as people age. Smokers have about a three times higher risk than nonsmokers. Even after quitting smoking, the risk remains elevated for a long time (at least 15 years).
 Laucoma, or green cataract, is a disease of the optic nerve. It often occurs because high eye pressure restricts the blood supply to the optic nerve. If you have glaucoma, parts of your visual field fall away. Untreated glaucoma can lead to blindness. Glaucoma is more common in smokers than in nonsmokers.
 Cataract or grey cataract is a condition in which the lens becomes cloudy. It can eventually lead to blindness. Grey cataracts are more common in smokers.</v>
       </c>
+      <c r="I17" t="str">
+        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+      </c>
       <c r="J17" t="str">
-        <v>https://www.ikstopnu.nl/bibliotheek/hoe-schadelijk-is-roken/#kanker</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K17" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L17" t="str">
         <v>Inspired by "Disease and death message themes" - text translated with deepl.</v>
       </c>
     </row>
@@ -881,23 +863,23 @@
       <c r="C18" t="str">
         <v>Antismoking ad - Sponge lungs</v>
       </c>
-      <c r="G18" t="str">
+      <c r="F18" t="str">
         <v>video</v>
       </c>
-      <c r="H18" t="str" xml:space="preserve">
+      <c r="G18" t="str" xml:space="preserve">
         <v xml:space="preserve">There is a video that showcases how smoking affects the lungs, which can be informative for you looking to quit smoking. I suggest you watch this video to gain a better understanding of the damaging effects of smoking on the lungs.
 Please be aware that the video may be difficult to watch, as it contains graphic images of damaged lungs. However, I understand that quitting smoking can be a challenging process, and gaining a better understanding of the harmful effects of smoking can be an important step in the right direction.
 https://youtu.be/htY_NBSyOk0
 After viewing the video, take a moment to reflect on what you learned and consider how it applies to your smoking habits. You may also find it helpful to jot down any insights or thoughts that come to mind while watching the video.
 </v>
       </c>
+      <c r="I18" t="str">
+        <v>TOP 40: SCARIEST ANTI-SMOKING COMMERCIALS [PART ONE]</v>
+      </c>
       <c r="J18" t="str">
-        <v>TOP 40: SCARIEST ANTI-SMOKING COMMERCIALS [PART ONE]</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K18" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L18" t="str">
         <v>Video resembling lung as a sponge that is black from smoking. Inspired by Pechmann's paper on using anti-smoking ads to convey severity. This ad is also considered very influencial based on Li-Ling Huang, Daniela B Friedman, Feng-Chang Lin, James F Thrasher, Which types of anti-smoking television advertisements work better in Taiwan?, Health Promotion International, Volume 33, Issue 3, June 2018, Pages 545–555, https://doi-org.tudelft.idm.oclc.org/10.1093/heapro/daw085</v>
       </c>
     </row>
@@ -912,21 +894,18 @@
         <v>Antismoking ad - Cigarettes are eating you alive</v>
       </c>
       <c r="F19" t="str">
-        <v>True</v>
-      </c>
-      <c r="G19" t="str">
         <v>video</v>
       </c>
-      <c r="H19" t="str" xml:space="preserve">
+      <c r="G19" t="str" xml:space="preserve">
         <v xml:space="preserve">Watching a video about the harmful effects of smoking on the body can be eye-opening and help motivate you to quit smoking. I recommend you watch the following video which explains the negative health impacts of smoking on the body.
 Please note that the recommended video contains some graphic images that may be difficult to watch. Nevertheless, it can be a helpful tool to motivate you to quit smoking and gain a better understanding of the negative health effects.  
 https://youtu.be/rmPAnIrSAMw
 After watching the video, take some time to reflect on what you learned and consider how it applies to your own life. It may also be helpful to jot down any insights or thoughts you have while watching the video.</v>
       </c>
-      <c r="J19" t="str">
+      <c r="I19" t="str">
         <v>TOP 40: SCARIEST ANTI-SMOKING COMMERCIALS [PART THREE]</v>
       </c>
-      <c r="L19" t="str">
+      <c r="K19" t="str">
         <v>Video showing the consequences in the body from smoking</v>
       </c>
     </row>
@@ -941,25 +920,22 @@
         <v>Antismoking ad - Personal stories anthem on the health consequences</v>
       </c>
       <c r="F20" t="str">
-        <v>True</v>
-      </c>
-      <c r="G20" t="str">
         <v>video</v>
       </c>
-      <c r="H20" t="str" xml:space="preserve">
+      <c r="G20" t="str" xml:space="preserve">
         <v xml:space="preserve">Gaining insight from other individuals about the negative effects tobacco had on their health can be beneficial when preparing to quit smoking.
 I thus recommend you watch the following short video with former smokers.
 The recommended video contains sensitive content about the negative effects of smoking on health. Despite this, it can be helpful to gain insight from the experiences of former smokers when preparing to quit.
 https://youtu.be/GEWky9PEroU
 After watching the video, consider what you can take away from these examples yourself. Type in some thoughts of what you think here.</v>
       </c>
+      <c r="I20" t="str">
+        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+      </c>
       <c r="J20" t="str">
-        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K20" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L20" t="str">
         <v>Video anthem of people that have health problems because of smoking. This video belongs to the scariest anti-smoking ads</v>
       </c>
     </row>
@@ -974,21 +950,18 @@
         <v>Writing about one's feared health consequences when not quitting smoking.</v>
       </c>
       <c r="F21" t="str">
-        <v>True</v>
-      </c>
-      <c r="G21" t="str">
         <v>activity</v>
       </c>
-      <c r="H21" t="str" xml:space="preserve">
+      <c r="G21" t="str" xml:space="preserve">
         <v xml:space="preserve">Having high motivation to quit smoking may aid in quitting successfully. 
 Thus, I advise you to think about who you do NOT want to be in the future but might become if you continue to smoke. 
 For example, you might NOT want to be a "mother who dies early of coronary heart disease as her mother did," a "husband who is frowned upon by his wife" or a "man who is dependent on a substance."</v>
       </c>
-      <c r="K21" t="str" xml:space="preserve">
+      <c r="J21" t="str" xml:space="preserve">
         <v xml:space="preserve">Michie, S., Brown, J., Geraghty, A. W., Miller, S., Yardley, L., Gardner, B., ... &amp; West, R. (2012). Development of StopAdvisor: a theory-based interactive internet-based smoking cessation intervention. Translational behavioral medicine, 2(3), 263-275.
 Albers, N., Neerincx, M. A., Penfornis, K. M., &amp; Brinkman, W. P. (2022). Users’ needs for a digital smoking cessation application and how to address them: A mixed-methods study. PeerJ, 10, e13824.</v>
       </c>
-      <c r="L21" t="str">
+      <c r="K21" t="str">
         <v>Inspired by preparatory activities no. 18 - PeerJ paper, Michie's paper on stopadvisor.</v>
       </c>
     </row>
@@ -1008,10 +981,10 @@
       <c r="E22" t="str">
         <v>50</v>
       </c>
-      <c r="G22" t="str">
+      <c r="F22" t="str">
         <v>video</v>
       </c>
-      <c r="H22" t="str" xml:space="preserve">
+      <c r="G22" t="str" xml:space="preserve">
         <v xml:space="preserve">Are you really aware of the health consquences if you continue smoking? 
 For that, I encourage you to watch a video to see the devastating effects of smoking and the importance of quitting. The video features Geri, who is battling with stage 4 cancer.
 It may be difficult to watch but can be helpful in understanding the devastating effects of smoking and the importance of quitting.
@@ -1019,13 +992,13 @@
 It can be difficult to confront the reality of the potential consequences of smoking, but seeing real-life experiences like Gary's can help motivate and inspire us to take action for our own health. Don't wait - watch now and take the first step towards a healthier future.
 </v>
       </c>
+      <c r="I22" t="str">
+        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+      </c>
       <c r="J22" t="str">
-        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K22" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L22" t="str">
         <v>Inspired by Pechmann, on showing personal stories videos for vulnerability. Video showing a woman (54) telling her experience living with Stage 4 COPD</v>
       </c>
     </row>
@@ -1045,22 +1018,22 @@
       <c r="E23" t="str">
         <v>50</v>
       </c>
-      <c r="G23" t="str">
+      <c r="F23" t="str">
         <v>video</v>
       </c>
-      <c r="H23" t="str" xml:space="preserve">
+      <c r="G23" t="str" xml:space="preserve">
         <v xml:space="preserve">For a better understanding of the health consequences of smoking, we encourage you to watch this video featuring Christine, who is battling oral cancer caused by smoking. 
 This video illustrates the devastating effects of smoking and the urgent importance of quitting. It can be tough to face the reality of the potential consequences of smoking, but seeing real-life experiences like Christine's can motivate and inspire us to take action for our health. 
 Here's the link to the video: 
 https://youtu.be/Yb0zDUzSktY</v>
       </c>
+      <c r="I23" t="str">
+        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+      </c>
       <c r="J23" t="str">
-        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K23" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L23" t="str">
         <v>Inspired by Pechmann, on showing personal stories videos for vulnerability. Video showing a woman (50s) telling her experience when she got oral cancer from smoking</v>
       </c>
     </row>
@@ -1080,23 +1053,23 @@
       <c r="E24" t="str">
         <v>40</v>
       </c>
-      <c r="G24" t="str">
+      <c r="F24" t="str">
         <v>video</v>
       </c>
-      <c r="H24" t="str" xml:space="preserve">
+      <c r="G24" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can have devasting health consequences.
 For that, I'd like to recommend a video featuring Brian, who suffered a stroke and experienced a slow recovery due to smoking. 
 Watching this video can help you understand the serious risks and potential consequences of smoking, as well as the impact it can have on your quality of life. Brian's story serves as a powerful reminder that smoking can lead to devastating health consequences, and I encourage you to watch the video to see for yourself. 
 Here's the link to the video: 
 https://youtu.be/juEHOkqeZ1I</v>
       </c>
+      <c r="I24" t="str">
+        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+      </c>
       <c r="J24" t="str">
-        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K24" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L24" t="str">
         <v>Inspired by Pechmann, on showing personal stories videos for vulnerability. Video showing a man (43) describing his experience of having a stroke casue by smoking and the consequences.</v>
       </c>
     </row>
@@ -1116,23 +1089,23 @@
       <c r="E25" t="str">
         <v>50</v>
       </c>
-      <c r="G25" t="str">
+      <c r="F25" t="str">
         <v>video</v>
       </c>
-      <c r="H25" t="str" xml:space="preserve">
+      <c r="G25" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can lead to severe and potentially life-threatening health consequences.
 I'd like to share a video with you featuring Michael, who began smoking at a very young age and later developed lung cancer. 
 This video highlights the serious health risks associated with smoking and the importance of quitting, particularly for those who start smoking at a young age. Michael's story is a powerful reminder that smoking can have long-lasting and life-threatening consequences, even for those who may not realize it at the time. 
 I encourage you to watch this video to learn more about the risks of smoking and the benefits of quitting. Here's the link to the video: 
 https://youtu.be/T1NusJTgBmI</v>
       </c>
+      <c r="I25" t="str">
+        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+      </c>
       <c r="J25" t="str">
-        <v>CDC: Tips from Former Smokers - Anthem Ad</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K25" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L25" t="str">
         <v>Inspired by Pechmann, on showing personal stories videos for vulnerability. Video showing a man (50s) describing how he started smoking when he was 9y old.</v>
       </c>
     </row>
@@ -1152,10 +1125,10 @@
       <c r="E26" t="str">
         <v>30</v>
       </c>
-      <c r="G26" t="str">
+      <c r="F26" t="str">
         <v>video</v>
       </c>
-      <c r="H26" t="str" xml:space="preserve">
+      <c r="G26" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking is associated with serious and potentially fatal health risks.
 I want to recommend a video that features a man who started smoking at a young age and has faced significant consequences as a result. This video highlights the long-term health effects of smoking and the impact it can have on your quality of life, regardless of your age. 
 Seeing the personal experiences of individuals like this man can serve as a powerful reminder of the risks associated with smoking and the importance of quitting. 
@@ -1163,13 +1136,13 @@
 Here's the link to the video: 
 https://youtu.be/Ebtn5lx8xms</v>
       </c>
+      <c r="I26" t="str">
+        <v>WHO</v>
+      </c>
       <c r="J26" t="str">
-        <v>WHO</v>
+        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
       </c>
       <c r="K26" t="str">
-        <v>Pechmann, C., Zhao, G., Goldberg, M. E., &amp; Reibling, E. T. (2003). What to convey in antismoking advertisements for adolescents: The use of protection motivation theory to identify effective message themes. Journal of marketing, 67(2), 1-18.</v>
-      </c>
-      <c r="L26" t="str">
         <v>Inspired by Pechmann, on showing personal stories videos for vulnerability. Video showing a man (30s) describing how he started smoking and then got sick and decided to stop.</v>
       </c>
     </row>
@@ -1184,12 +1157,9 @@
         <v>Young smokers are less physically strong than young non-smokers</v>
       </c>
       <c r="F27" t="str">
-        <v>True</v>
-      </c>
-      <c r="G27" t="str">
-        <v>text</v>
-      </c>
-      <c r="H27" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G27" t="str" xml:space="preserve">
         <v xml:space="preserve">Did you know that smokers are have less physical strength than non-smokers?
 yes;no</v>
       </c>
@@ -1204,18 +1174,18 @@
       <c r="C28" t="str">
         <v>Young smokers are less physically strong than young non-smokers</v>
       </c>
-      <c r="G28" t="str">
-        <v>text</v>
-      </c>
-      <c r="H28" t="str" xml:space="preserve">
+      <c r="F28" t="str">
+        <v>text</v>
+      </c>
+      <c r="G28" t="str" xml:space="preserve">
         <v xml:space="preserve">If you're looking for reasons to quit smoking, consider this: according to recent research, smoking may be making you weaker, both physically and socially. 
 The study was conducted among male smokers and non-smokers 18-27 years old and found that smokers had less physical strength than nonsmokers, and that young smokers showed a decrease in physical activity skills. 
 This means that smoking could be robbing you of your personal and social power over time, leaving you with a weaker, less active lifestyle. So if you want to be your strongest, most powerful self, it's time to kick the habit and start living smoke-free.</v>
       </c>
-      <c r="J28" t="str">
+      <c r="I28" t="str">
         <v>Moslemi-Haghighi F, Rezaei I, Ghaffarinejad F, Lari R, Pouya F. Comparison of Physical Fitness among Smoker and Non-Smoker Men. Addict Health. 2011 Winter-Spring;3(1-2):15-9. PMID: 24494112; PMCID: PMC3905518.</v>
       </c>
-      <c r="L28" t="str">
+      <c r="K28" t="str">
         <v>ony for young (18-27) men - text adapted by chatGPT 16/3/2023</v>
       </c>
     </row>
@@ -1230,16 +1200,13 @@
         <v>Smokers are more likely to get lung cancer than non-smokers</v>
       </c>
       <c r="F29" t="str">
-        <v>True</v>
-      </c>
-      <c r="G29" t="str">
-        <v>text</v>
-      </c>
-      <c r="H29" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G29" t="str" xml:space="preserve">
         <v xml:space="preserve">Do you know how many times it is more likely for smokers to get lung cancer compared to non-smokers?
 2;10;15</v>
       </c>
-      <c r="J29" t="str">
+      <c r="I29" t="str">
         <v>https://www.cdc.gov/cancer/lung/basic_info/risk_factors.htm</v>
       </c>
     </row>
@@ -1253,14 +1220,14 @@
       <c r="C30" t="str">
         <v>Smokers are more likely to get lung cancer than non-smokers</v>
       </c>
-      <c r="G30" t="str">
-        <v>text</v>
-      </c>
-      <c r="H30" t="str" xml:space="preserve">
+      <c r="F30" t="str">
+        <v>text</v>
+      </c>
+      <c r="G30" t="str" xml:space="preserve">
         <v xml:space="preserve">People who smoke cigarettes are 15 to 30 times more likely to get lung cancer or die from lung cancer than people who do not smoke. Even smoking a few cigarettes a day or smoking occasionally increases the risk of lung cancer. The more years a person smokes and the more cigarettes smoked each day, the more risk goes up.
 People who quit smoking have a lower risk of lung cancer than if they had continued to smoke, but their risk is higher than the risk for people who never smoked. Quitting smoking at any age can lower the risk of lung cancer.</v>
       </c>
-      <c r="J30" t="str">
+      <c r="I30" t="str">
         <v>https://www.cdc.gov/cancer/lung/basic_info/risk_factors.htm</v>
       </c>
     </row>
@@ -1274,10 +1241,10 @@
       <c r="C31" t="str">
         <v>Women smokers have less changes getting pregnant than non-smokers</v>
       </c>
-      <c r="G31" t="str">
-        <v>text</v>
-      </c>
-      <c r="H31" t="str" xml:space="preserve">
+      <c r="F31" t="str">
+        <v>text</v>
+      </c>
+      <c r="G31" t="str" xml:space="preserve">
         <v xml:space="preserve">
 How much is the infertility rate between female smokers and nonsmokers?
 half;about the same;double</v>
@@ -1297,23 +1264,20 @@
         <v>woman</v>
       </c>
       <c r="F32" t="str">
-        <v>True</v>
-      </c>
-      <c r="G32" t="str">
-        <v>text</v>
-      </c>
-      <c r="H32" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G32" t="str" xml:space="preserve">
         <v xml:space="preserve">If you're a woman who is trying to conceive, it's important to know that smoking can have a significant impact on your fertility. Studies have shown that female smokers are less efficient at conceiving than nonsmokers, and that infertility rates in both male and female smokers are about twice the rate found in nonsmokers.
 Even if you are undergoing fertility treatments such as IVF, smoking can still have a negative impact on your chances of getting pregnant. In fact, female smokers undergoing IVF require more ovary-stimulating medications and have fewer eggs at retrieval time, resulting in lower pregnancy rates compared to IVF patients who do not smoke.</v>
       </c>
-      <c r="I32" t="str" xml:space="preserve">
+      <c r="H32" t="str" xml:space="preserve">
         <v xml:space="preserve">Smoking can damage the genetic material in eggs and sperm, leading to higher rates (double) of miscarriage and offspring birth-defects. Women who smoke are also more likely to conceive a chromosomally unhealthy pregnancy, such as one affected by Down syndrome. And if you do manage to get pregnant, you may be at a higher risk for ectopic pregnancies and preterm labor.
 The good news is that quitting smoking can improve your fertility and decrease your risk of pregnancy complications. While the decrease in egg supply cannot be reversed, the rate of pregnancy complications due to smoking decreases the longer you stay smoke-free. So if you're trying to conceive, the best thing you can do is quit smoking as soon as possible to give yourself the best chance of having a healthy, successful pregnancy.</v>
       </c>
-      <c r="J32" t="str">
+      <c r="I32" t="str">
         <v>https://www.reproductivefacts.org/news-and-publications/patient-fact-sheets-and-booklets/documents/fact-sheets-and-info-booklets/smoking-and-infertility/#:~:text=Infertility%20rates%20in%20both%20male,number%20of%20cigarettes%20smoked%20daily.</v>
       </c>
-      <c r="L32" t="str">
+      <c r="K32" t="str">
         <v>only for women - text adapted by chatGPT 16/3/2023</v>
       </c>
     </row>
@@ -1328,26 +1292,23 @@
         <v>Personal rule for becoming more physically active</v>
       </c>
       <c r="F33" t="str">
-        <v>True</v>
-      </c>
-      <c r="G33" t="str">
-        <v>text</v>
-      </c>
-      <c r="H33" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G33" t="str" xml:space="preserve">
         <v xml:space="preserve">Being more physically active (e.g., taking walks, swimming, or going running) may aid you to stop smoking. 
 One important aspect for this is to have strong resolve to become more physically active. 
 So, I advise you to take some time to think and create a personal rule that helps you to become more physically active. 
 Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." 
 Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</v>
       </c>
-      <c r="J33" t="str">
+      <c r="I33" t="str">
         <v>PeerJ paper, Michie's paper on stopadvisor.</v>
       </c>
-      <c r="K33" t="str" xml:space="preserve">
+      <c r="J33" t="str" xml:space="preserve">
         <v xml:space="preserve">Michie, S., Brown, J., Geraghty, A. W., Miller, S., Yardley, L., Gardner, B., ... &amp; West, R. (2012). Development of StopAdvisor: a theory-based interactive internet-based smoking cessation intervention. Translational behavioral medicine, 2(3), 263-275.
 Albers, N., Neerincx, M. A., Penfornis, K. M., &amp; Brinkman, W. P. (2022). Users’ needs for a digital smoking cessation application and how to address them: A mixed-methods study. PeerJ, 10, e13824</v>
       </c>
-      <c r="L33" t="str">
+      <c r="K33" t="str">
         <v>Taken from preparatory activities 9</v>
       </c>
     </row>
@@ -1362,20 +1323,17 @@
         <v>Plan for becoming more physically active</v>
       </c>
       <c r="F34" t="str">
-        <v>True</v>
-      </c>
-      <c r="G34" t="str">
         <v>activity</v>
       </c>
-      <c r="H34" t="str" xml:space="preserve">
+      <c r="G34" t="str" xml:space="preserve">
         <v xml:space="preserve">Becoming more physically active (e.g., taking walks, dancing, swimming) may help you to successfully quit smoking. 
 One crucial part for this is to create a plan for becoming more physically active. Therefore, I advise you to think about what you could do to become more physically active. 
 For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Type in everything that comes to your mind. Which plan do you want to focus on?</v>
       </c>
+      <c r="J34" t="str">
+        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
+      </c>
       <c r="K34" t="str">
-        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
-      </c>
-      <c r="L34" t="str">
         <v>Taken from preparatory activities 41 - In line with action-planning</v>
       </c>
     </row>
@@ -1390,27 +1348,24 @@
         <v>Focusing on past successes for becoming more physically active</v>
       </c>
       <c r="F35" t="str">
-        <v>True</v>
-      </c>
-      <c r="G35" t="str">
         <v>activity</v>
       </c>
-      <c r="H35" t="str" xml:space="preserve">
+      <c r="G35" t="str" xml:space="preserve">
         <v xml:space="preserve">To increase your confidence that you will succeed in becoming more physically active and changing your behavior, it can help to think back to previous successes. 
 Take a moment to reflect on times when you succeeded in something or felt satisfied. Have you ever won a competition? Did you cook something delicious recently? Or maybe you learned a new language? 
 Start writing here and make a list of your success moments. No success is too small to write down! Take a few minutes to make your list before sending it. Then take a closer look at your list. Try to think about what helped you to achieve your success. 
 If you want, write down your list on paper so you do not forget it. You can also hang or place your list somewhere in your home so that you are reminded of your successes more often. The list shows that you can be proud of yourself.</v>
       </c>
-      <c r="J35" t="str" xml:space="preserve">
+      <c r="I35" t="str" xml:space="preserve">
         <v xml:space="preserve">https://www.stichtingstopbewust.nl/
 Perfect Fit: https://perfectfit-research.com/
 Michie, S., Ashford, S., Sniehotta, FalkoF., Dombrowski, StephanU., Bishop, A., &amp; French, DavidP. (2011). A refined taxonomy of behaviour change techniques to help people change their physical activity and healthy eating behaviours: The CALO-RE taxonomy. Psychology &amp; Health, 26(11), 1479–1498. https://doi.org/10.1080/08870446.2010.540664</v>
       </c>
-      <c r="K35" t="str" xml:space="preserve">
+      <c r="J35" t="str" xml:space="preserve">
         <v xml:space="preserve">"Based on Perfect Fit bible status 27-2-2023, activity C2.4, this in turn is based on: https://www.stichtingstopbewust.nl/ and the paper from Michie below.
 Michie, S., Ashford, S., Sniehotta, FalkoF., Dombrowski, StephanU., Bishop, A., &amp; French, DavidP. (2011). A refined taxonomy of behaviour change techniques to help people change their physical activity and healthy eating behaviours: The CALO-RE taxonomy. Psychology &amp; Health, 26(11), 1479–1498. https://doi.org/10.1080/08870446.2010.540664"</v>
       </c>
-      <c r="L35" t="str">
+      <c r="K35" t="str">
         <v>Taken from preparatory activities 43 - In line with feedback on past experiences</v>
       </c>
     </row>
@@ -1425,24 +1380,21 @@
         <v>Testimonial on becoming more physically active</v>
       </c>
       <c r="F36" t="str">
-        <v>True</v>
-      </c>
-      <c r="G36" t="str">
         <v>video</v>
       </c>
-      <c r="H36" t="str" xml:space="preserve">
+      <c r="G36" t="str" xml:space="preserve">
         <v xml:space="preserve">When preparing for becoming more physically active, it can be useful to learn from other people who have succeeded in becoming more physically active. 
 What goal did they set for themselves? And how did they reach it? 
 I  recommend you watch this short video in which 5 people describe how they reached their physical activity goals: 
 https://youtu.be/m1MHo9fCTG8. 
 What can you take away from the 5 examples for yourself?</v>
       </c>
-      <c r="J36" t="str" xml:space="preserve">
+      <c r="I36" t="str" xml:space="preserve">
         <v xml:space="preserve">"Albers, N., Hizli, B., Scheltinga, B. L., Meijer, E., &amp; Brinkman, W. P. (2023). Setting Physical Activity Goals with a Virtual Coach: Vicarious Experiences, Personalization and Acceptance. Journal of Medical Systems, 47(1), 15.
 Hizli, B., Albers, N., &amp; Brinkman, W.-P. (2022). Data and code underlying the master thesis: Goal-setting dialogue for physical activity with a virtual coach (Version 1). 4TU.ResearchData. https://doi.org/10.4121/20047328.v1
 "</v>
       </c>
-      <c r="L36" t="str">
+      <c r="K36" t="str">
         <v>Taken from preparatory activity 3</v>
       </c>
     </row>
@@ -1457,21 +1409,18 @@
         <v>Thinking of a passive activity that one could exchange for an active activity. For example, taking the stairs instead of the elevator.</v>
       </c>
       <c r="F37" t="str">
-        <v>True</v>
-      </c>
-      <c r="G37" t="str">
         <v>activity</v>
       </c>
-      <c r="H37" t="str" xml:space="preserve">
+      <c r="G37" t="str" xml:space="preserve">
         <v xml:space="preserve">Becoming more physically active (e.g., taking walks, running, swimming) may help you successfully quit smoking. 
 One crucial part of this is thinking about ways to incorporate physical activity into your daily life. One way to do this is to exchange a passive activity for an active one. Therefore, I advise you to take a moment and think about ways you could exchange a passive activity for an active one. 
 For example, you could take the stairs instead of the escalator, bike to work instead of taking the bus, or work at a standing desk. 
 Start typing in everything that comes to your mind. Which exchange do you want to focus on? </v>
       </c>
+      <c r="J37" t="str">
+        <v>Inspiration from https://www.voedingscentrum.nl/nl/thema/eetwissel/zo-maak-je-een-eigen-eetwissel.aspx</v>
+      </c>
       <c r="K37" t="str">
-        <v>Inspiration from https://www.voedingscentrum.nl/nl/thema/eetwissel/zo-maak-je-een-eigen-eetwissel.aspx</v>
-      </c>
-      <c r="L37" t="str">
         <v>Taken from preparatory activities 37</v>
       </c>
     </row>
@@ -1486,12 +1435,9 @@
         <v>Plan for PA</v>
       </c>
       <c r="F38" t="str">
-        <v>True</v>
-      </c>
-      <c r="G38" t="str">
-        <v>text</v>
-      </c>
-      <c r="H38" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G38" t="str" xml:space="preserve">
         <v xml:space="preserve">Exercise is perfect for your health. And this does not mean you always have to be completely exhausted after exercising. It's more important to exercise regularly (Benefits of exercise - NHS (www.nhs.uk) and have fun doing so.
 Therefore, find an activity that you enjoy.
 What do you like to do?
@@ -1508,14 +1454,14 @@
       <c r="C39" t="str">
         <v>Plan for PA</v>
       </c>
-      <c r="G39" t="str">
-        <v>text</v>
-      </c>
-      <c r="H39" t="str" xml:space="preserve">
+      <c r="F39" t="str">
+        <v>text</v>
+      </c>
+      <c r="G39" t="str" xml:space="preserve">
         <v xml:space="preserve">If you like walking, cycling, or going for a run, you can find great routes on the internet. For example, at: 
 https://www.strava.com/</v>
       </c>
-      <c r="J39" t="str" xml:space="preserve">
+      <c r="I39" t="str" xml:space="preserve">
         <v xml:space="preserve">https://www.nhs.uk/live-well/exercise/exercise-health-benefits/
 heart.org
 https://sport.nl/sportwijzer
@@ -1525,10 +1471,10 @@
 runnersmap.nl
 supportervanallehardlopers.nl/hardloopplanner/start</v>
       </c>
+      <c r="J39" t="str">
+        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
+      </c>
       <c r="K39" t="str">
-        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
-      </c>
-      <c r="L39" t="str">
         <v>In line with providing instructions on how to achieve an activity - Taken from PF Bible - C2 resources</v>
       </c>
     </row>
@@ -1542,14 +1488,14 @@
       <c r="C40" t="str">
         <v>Plan for PA</v>
       </c>
-      <c r="G40" t="str">
-        <v>text</v>
-      </c>
-      <c r="H40" t="str" xml:space="preserve">
+      <c r="F40" t="str">
+        <v>text</v>
+      </c>
+      <c r="G40" t="str" xml:space="preserve">
         <v xml:space="preserve">If you prefer to do some fitness exercises at home, you might want to check out these exercises: 
 https://blog.myfitnesspal.com/10-minute-no-equipment-total-body-workout/</v>
       </c>
-      <c r="J40" t="str" xml:space="preserve">
+      <c r="I40" t="str" xml:space="preserve">
         <v xml:space="preserve">https://www.nhs.uk/live-well/exercise/exercise-health-benefits/
 heart.org
 https://sport.nl/sportwijzer
@@ -1559,10 +1505,10 @@
 runnersmap.nl
 supportervanallehardlopers.nl/hardloopplanner/start</v>
       </c>
+      <c r="J40" t="str">
+        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
+      </c>
       <c r="K40" t="str">
-        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
-      </c>
-      <c r="L40" t="str">
         <v>In line with providing instructions on how to achieve an activity - Taken from PF Bible - C2 resources</v>
       </c>
     </row>
@@ -1576,14 +1522,14 @@
       <c r="C41" t="str">
         <v>Plan for PA</v>
       </c>
-      <c r="G41" t="str">
-        <v>text</v>
-      </c>
-      <c r="H41" t="str" xml:space="preserve">
+      <c r="F41" t="str">
+        <v>text</v>
+      </c>
+      <c r="G41" t="str" xml:space="preserve">
         <v xml:space="preserve">Besides cycling, walking, and fitness, there are many other activities to get moving. Just go to https://www.bbc.com/news/uk-28062001. Fill in the sports guide questions and see which sports suit you. Moreover, it is helpful to alternate activities. That way, exercise never gets boring (heart.org).
 Have you found a sport you like? Then I recommend you to check the clubs or associations nearby you. This way, you can not only play sports but also get to know other people. After all, it's easier to stick to a sport if you have company (heart.org)!</v>
       </c>
-      <c r="J41" t="str" xml:space="preserve">
+      <c r="I41" t="str" xml:space="preserve">
         <v xml:space="preserve">https://www.nhs.uk/live-well/exercise/exercise-health-benefits/
 heart.org
 https://sport.nl/sportwijzer
@@ -1593,10 +1539,10 @@
 runnersmap.nl
 supportervanallehardlopers.nl/hardloopplanner/start</v>
       </c>
+      <c r="J41" t="str">
+        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
+      </c>
       <c r="K41" t="str">
-        <v>S. L. Williams, D. P. French, What are the most effective intervention techniques for changing physical activity self-efficacy and physical activity behaviour—and are they the same?, Health Education Research, Volume 26, Issue 2, April 2011, Pages 308–322, https://doi.org/10.1093/her/cyr005</v>
-      </c>
-      <c r="L41" t="str">
         <v>In line with providing instructions on how to achieve an activity - Taken from PF Bible - C2 resources</v>
       </c>
     </row>
@@ -1610,18 +1556,18 @@
       <c r="C42" t="str">
         <v>Personal testimonials</v>
       </c>
-      <c r="G42" t="str">
+      <c r="F42" t="str">
         <v>video</v>
       </c>
-      <c r="H42" t="str" xml:space="preserve">
+      <c r="G42" t="str" xml:space="preserve">
         <v xml:space="preserve">Engaging in physical activity can be beneficial in the process of quitting smoking.
 To aid increasing your physical activity, I recommend you to watch this short video featuring people who have experienced the positive effects of exercise. From walking to the shops instead of driving to doing yoga and housework, there are countless ways to incorporate physical activity into your daily routine. 
 Get motivated by these examples and start making small changes today to improve your overall health and wellbeing.</v>
       </c>
-      <c r="J42" t="str">
+      <c r="I42" t="str">
         <v>Previous study material (testimonials)</v>
       </c>
-      <c r="L42" t="str">
+      <c r="K42" t="str">
         <v>Text and script developed by chatGPT - 20/3/2023</v>
       </c>
     </row>
@@ -1636,22 +1582,19 @@
         <v>PA video on cravings</v>
       </c>
       <c r="F43" t="str">
-        <v>True</v>
-      </c>
-      <c r="G43" t="str">
         <v>video</v>
       </c>
-      <c r="H43" t="str" xml:space="preserve">
+      <c r="G43" t="str" xml:space="preserve">
         <v xml:space="preserve">Becoming more physically active (e.g., swimming, taking walks, boxing) may help you to successfully quit smoking. 
 One crucial step for this is to have high aspiration to become more physically active. 
 So, I advise you to watch the following short video about the possible positive impact of physical activity on dealing with cravings to smoke: 
 https://youtu.be/iakhFA-jPCc. 
 What do you think about the information in the video?</v>
       </c>
-      <c r="J43" t="str">
+      <c r="I43" t="str">
         <v>G3_PA_Cravings video</v>
       </c>
-      <c r="L43" t="str">
+      <c r="K43" t="str">
         <v xml:space="preserve">Taken from preparatory activities 38 </v>
       </c>
     </row>
@@ -1666,21 +1609,18 @@
         <v>PA video on quit smoking in general</v>
       </c>
       <c r="F44" t="str">
-        <v>True</v>
-      </c>
-      <c r="G44" t="str">
         <v>video</v>
       </c>
-      <c r="H44" t="str" xml:space="preserve">
+      <c r="G44" t="str" xml:space="preserve">
         <v xml:space="preserve">Physical activity helps to quit smoking. 
 To understand why, I suggest watching this short video: 
 https://youtu.be/qoD2j_lTm9U. 
 How do you think can physical activity help you to quit smoking? </v>
       </c>
-      <c r="J44" t="str">
+      <c r="I44" t="str">
         <v>U7 - PA helps quit smoking</v>
       </c>
-      <c r="L44" t="str">
+      <c r="K44" t="str">
         <v>Taken from preparatory activities 50</v>
       </c>
     </row>
@@ -1695,12 +1635,9 @@
         <v>PA is good for you 1</v>
       </c>
       <c r="F45" t="str">
-        <v>True</v>
-      </c>
-      <c r="G45" t="str">
-        <v>text</v>
-      </c>
-      <c r="H45" t="str" xml:space="preserve">
+        <v>text</v>
+      </c>
+      <c r="G45" t="str" xml:space="preserve">
         <v xml:space="preserve">Did you know that physical activity provides numerous health benefits, and it can also help you quit smoking?
 yes;no</v>
       </c>
@@ -1715,16 +1652,16 @@
       <c r="C46" t="str">
         <v>PA is good for you 1</v>
       </c>
-      <c r="G46" t="str">
-        <v>text</v>
-      </c>
-      <c r="H46" t="str" xml:space="preserve">
+      <c r="F46" t="str">
+        <v>text</v>
+      </c>
+      <c r="G46" t="str" xml:space="preserve">
         <v xml:space="preserve">Quiting smoking can be hard and starting a regular exercise routine may be the key to your success! 
 Exercise helps to reduce cravings and withdrawal symptoms, while also providing a healthy outlet for stress and anxiety. 
 By incorporating regular physical activity into your daily routine, you may find it easier to quit smoking and stay smoke-free for the long-term. So why not give it a try? 
 Believe in yourself and your ability to make positive changes in your life. With commitment and dedication, you can achieve your health and wellness goals. Start working out today and see the positive impact it can have on your life!</v>
       </c>
-      <c r="L46" t="str">
+      <c r="K46" t="str">
         <v>text generated by chatGPT 21/3/2023</v>
       </c>
     </row>
@@ -1738,16 +1675,16 @@
       <c r="C47" t="str">
         <v>Expert's testimonial</v>
       </c>
+      <c r="F47" t="str">
+        <v>text</v>
+      </c>
       <c r="G47" t="str">
-        <v>text</v>
-      </c>
-      <c r="H47" t="str">
         <v>Eline's testimonial</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L47"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K47"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>